<commit_message>
generatos file, hydro data
</commit_message>
<xml_diff>
--- a/PNW_generators.xlsx
+++ b/PNW_generators.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1082" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1097" uniqueCount="318">
   <si>
     <t>name</t>
   </si>
@@ -968,6 +968,24 @@
   </si>
   <si>
     <t>&lt;----CF</t>
+  </si>
+  <si>
+    <t>P3I</t>
+  </si>
+  <si>
+    <t>P8I</t>
+  </si>
+  <si>
+    <t>P14I</t>
+  </si>
+  <si>
+    <t>P65I</t>
+  </si>
+  <si>
+    <t>P66I</t>
+  </si>
+  <si>
+    <t>imports</t>
   </si>
 </sst>
 </file>
@@ -3638,10 +3656,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T96"/>
+  <dimension ref="A1:T101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="O96" sqref="O96"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="A100" sqref="A100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9257,13 +9275,13 @@
         <v>1200</v>
       </c>
       <c r="G96" s="4">
-        <v>8.5491119346179705</v>
+        <v>10</v>
       </c>
       <c r="H96" s="4">
-        <v>8.6141366967335706</v>
+        <v>10</v>
       </c>
       <c r="I96" s="4">
-        <v>8.6791614588491708</v>
+        <v>10</v>
       </c>
       <c r="J96" s="4">
         <v>300</v>
@@ -9280,7 +9298,7 @@
       <c r="N96">
         <v>3.17</v>
       </c>
-      <c r="O96">
+      <c r="O96" s="4">
         <v>505.60567200000202</v>
       </c>
       <c r="P96">
@@ -9295,6 +9313,196 @@
       </c>
       <c r="S96" t="s">
         <v>311</v>
+      </c>
+    </row>
+    <row r="97" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>312</v>
+      </c>
+      <c r="D97" t="s">
+        <v>317</v>
+      </c>
+      <c r="E97" t="s">
+        <v>13</v>
+      </c>
+      <c r="G97">
+        <v>0</v>
+      </c>
+      <c r="H97">
+        <v>0</v>
+      </c>
+      <c r="I97">
+        <v>0</v>
+      </c>
+      <c r="J97">
+        <v>0</v>
+      </c>
+      <c r="L97">
+        <v>1</v>
+      </c>
+      <c r="M97">
+        <v>1</v>
+      </c>
+      <c r="N97">
+        <v>0</v>
+      </c>
+      <c r="O97">
+        <v>0</v>
+      </c>
+      <c r="P97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>313</v>
+      </c>
+      <c r="D98" t="s">
+        <v>317</v>
+      </c>
+      <c r="E98" t="s">
+        <v>13</v>
+      </c>
+      <c r="G98">
+        <v>0</v>
+      </c>
+      <c r="H98">
+        <v>0</v>
+      </c>
+      <c r="I98">
+        <v>0</v>
+      </c>
+      <c r="J98">
+        <v>0</v>
+      </c>
+      <c r="L98">
+        <v>1</v>
+      </c>
+      <c r="M98">
+        <v>1</v>
+      </c>
+      <c r="N98">
+        <v>0</v>
+      </c>
+      <c r="O98">
+        <v>0</v>
+      </c>
+      <c r="P98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>314</v>
+      </c>
+      <c r="D99" t="s">
+        <v>317</v>
+      </c>
+      <c r="E99" t="s">
+        <v>13</v>
+      </c>
+      <c r="G99">
+        <v>0</v>
+      </c>
+      <c r="H99">
+        <v>0</v>
+      </c>
+      <c r="I99">
+        <v>0</v>
+      </c>
+      <c r="J99">
+        <v>0</v>
+      </c>
+      <c r="L99">
+        <v>1</v>
+      </c>
+      <c r="M99">
+        <v>1</v>
+      </c>
+      <c r="N99">
+        <v>0</v>
+      </c>
+      <c r="O99">
+        <v>0</v>
+      </c>
+      <c r="P99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>315</v>
+      </c>
+      <c r="D100" t="s">
+        <v>317</v>
+      </c>
+      <c r="E100" t="s">
+        <v>13</v>
+      </c>
+      <c r="G100">
+        <v>0</v>
+      </c>
+      <c r="H100">
+        <v>0</v>
+      </c>
+      <c r="I100">
+        <v>0</v>
+      </c>
+      <c r="J100">
+        <v>0</v>
+      </c>
+      <c r="L100">
+        <v>1</v>
+      </c>
+      <c r="M100">
+        <v>1</v>
+      </c>
+      <c r="N100">
+        <v>0</v>
+      </c>
+      <c r="O100">
+        <v>0</v>
+      </c>
+      <c r="P100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>316</v>
+      </c>
+      <c r="D101" t="s">
+        <v>317</v>
+      </c>
+      <c r="E101" t="s">
+        <v>13</v>
+      </c>
+      <c r="G101">
+        <v>0</v>
+      </c>
+      <c r="H101">
+        <v>0</v>
+      </c>
+      <c r="I101">
+        <v>0</v>
+      </c>
+      <c r="J101">
+        <v>0</v>
+      </c>
+      <c r="L101">
+        <v>1</v>
+      </c>
+      <c r="M101">
+        <v>1</v>
+      </c>
+      <c r="N101">
+        <v>0</v>
+      </c>
+      <c r="O101">
+        <v>0</v>
+      </c>
+      <c r="P101">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add paths data to generators file
</commit_message>
<xml_diff>
--- a/PNW_generators.xlsx
+++ b/PNW_generators.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joy Hill\Desktop\BPA_stuff\PNW_Dispatch\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sdenaro\OneDrive - University of North Carolina at Chapel Hill\UNC_2017\Dispatch_model\PNW_Dispatch\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9190" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,6 +31,40 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Lenovo User</author>
+  </authors>
+  <commentList>
+    <comment ref="A101" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Lenovo User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Maybe path 66 shouldn't be here because it's only exports</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1097" uniqueCount="318">
   <si>
@@ -992,7 +1026,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1029,6 +1063,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1050,7 +1097,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1065,6 +1112,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1643,7 +1691,7 @@
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns="" Requires="cx1">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="2" name="Chart 1"/>
@@ -1663,7 +1711,7 @@
       <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="2" name="Rectangle 1"/>
+            <xdr:cNvPr id="0" name=""/>
             <xdr:cNvSpPr>
               <a:spLocks noTextEdit="1"/>
             </xdr:cNvSpPr>
@@ -1969,12 +2017,12 @@
       <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.21875" customWidth="1"/>
+    <col min="1" max="1" width="25.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2018,7 +2066,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -2032,7 +2080,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -2046,7 +2094,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -2060,7 +2108,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -2074,7 +2122,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -2088,7 +2136,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -2102,7 +2150,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -2116,7 +2164,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -2130,7 +2178,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -2144,7 +2192,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -2158,7 +2206,7 @@
         <v>30.9</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -2172,7 +2220,7 @@
         <v>30.9</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -2186,7 +2234,7 @@
         <v>179.4</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -2200,7 +2248,7 @@
         <v>122.1</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -2214,7 +2262,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -2228,7 +2276,7 @@
         <v>301.5</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -2242,7 +2290,7 @@
         <v>10.9</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -2256,7 +2304,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -2270,7 +2318,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -2284,7 +2332,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -2298,7 +2346,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -2312,7 +2360,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>37</v>
       </c>
@@ -2326,7 +2374,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>38</v>
       </c>
@@ -2340,7 +2388,7 @@
         <v>729.9</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -2354,7 +2402,7 @@
         <v>729.9</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>40</v>
       </c>
@@ -2368,7 +2416,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>41</v>
       </c>
@@ -2382,7 +2430,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>42</v>
       </c>
@@ -2396,7 +2444,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>43</v>
       </c>
@@ -2410,7 +2458,7 @@
         <v>1170</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>44</v>
       </c>
@@ -2424,7 +2472,7 @@
         <v>124.65</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>45</v>
       </c>
@@ -2438,7 +2486,7 @@
         <v>144.35</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>46</v>
       </c>
@@ -2452,7 +2500,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>47</v>
       </c>
@@ -2466,7 +2514,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>48</v>
       </c>
@@ -2480,7 +2528,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>49</v>
       </c>
@@ -2494,7 +2542,7 @@
         <v>212.5</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>50</v>
       </c>
@@ -2508,7 +2556,7 @@
         <v>212.5</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>51</v>
       </c>
@@ -2522,7 +2570,7 @@
         <v>264.39999999999998</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>52</v>
       </c>
@@ -2536,7 +2584,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>53</v>
       </c>
@@ -2550,7 +2598,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>54</v>
       </c>
@@ -2564,7 +2612,7 @@
         <v>161.5</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>55</v>
       </c>
@@ -2578,7 +2626,7 @@
         <v>161.5</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>56</v>
       </c>
@@ -2592,7 +2640,7 @@
         <v>178.5</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>57</v>
       </c>
@@ -2606,7 +2654,7 @@
         <v>29.4</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>58</v>
       </c>
@@ -2620,7 +2668,7 @@
         <v>29.4</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>59</v>
       </c>
@@ -2634,7 +2682,7 @@
         <v>29.4</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>60</v>
       </c>
@@ -2648,7 +2696,7 @@
         <v>29.4</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>61</v>
       </c>
@@ -2662,7 +2710,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>62</v>
       </c>
@@ -2676,7 +2724,7 @@
         <v>11.4</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>63</v>
       </c>
@@ -2690,7 +2738,7 @@
         <v>11.4</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>64</v>
       </c>
@@ -2704,7 +2752,7 @@
         <v>11.4</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>65</v>
       </c>
@@ -2718,7 +2766,7 @@
         <v>11.4</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>66</v>
       </c>
@@ -2732,7 +2780,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>67</v>
       </c>
@@ -2746,7 +2794,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>68</v>
       </c>
@@ -2760,7 +2808,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>69</v>
       </c>
@@ -2774,7 +2822,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>70</v>
       </c>
@@ -2788,7 +2836,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>71</v>
       </c>
@@ -2802,7 +2850,7 @@
         <v>-166</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>72</v>
       </c>
@@ -2816,7 +2864,7 @@
         <v>-166</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>73</v>
       </c>
@@ -2830,7 +2878,7 @@
         <v>-166</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>74</v>
       </c>
@@ -2844,7 +2892,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>75</v>
       </c>
@@ -2858,7 +2906,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>76</v>
       </c>
@@ -2872,7 +2920,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>77</v>
       </c>
@@ -2886,7 +2934,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>78</v>
       </c>
@@ -2900,7 +2948,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>79</v>
       </c>
@@ -2914,7 +2962,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>80</v>
       </c>
@@ -2928,7 +2976,7 @@
         <v>689.4</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>81</v>
       </c>
@@ -2942,7 +2990,7 @@
         <v>501.5</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>82</v>
       </c>
@@ -2956,7 +3004,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>83</v>
       </c>
@@ -2970,7 +3018,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>84</v>
       </c>
@@ -2984,7 +3032,7 @@
         <v>106.1</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>85</v>
       </c>
@@ -2998,7 +3046,7 @@
         <v>204.5</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>86</v>
       </c>
@@ -3012,7 +3060,7 @@
         <v>106.1</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>87</v>
       </c>
@@ -3026,7 +3074,7 @@
         <v>204.5</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>88</v>
       </c>
@@ -3046,7 +3094,7 @@
         <v>1956261</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>89</v>
       </c>
@@ -3060,7 +3108,7 @@
         <v>310.60000000000002</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>90</v>
       </c>
@@ -3074,7 +3122,7 @@
         <v>68.3</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>91</v>
       </c>
@@ -3088,7 +3136,7 @@
         <v>68.3</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>92</v>
       </c>
@@ -3102,7 +3150,7 @@
         <v>68.3</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>93</v>
       </c>
@@ -3116,7 +3164,7 @@
         <v>68.3</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>94</v>
       </c>
@@ -3130,7 +3178,7 @@
         <v>68.3</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>95</v>
       </c>
@@ -3144,7 +3192,7 @@
         <v>68.3</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>96</v>
       </c>
@@ -3158,7 +3206,7 @@
         <v>176.4</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>97</v>
       </c>
@@ -3172,7 +3220,7 @@
         <v>642.20000000000005</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>98</v>
       </c>
@@ -3186,7 +3234,7 @@
         <v>185.8</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>99</v>
       </c>
@@ -3200,7 +3248,7 @@
         <v>80.599999999999994</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>100</v>
       </c>
@@ -3214,7 +3262,7 @@
         <v>62.2</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>101</v>
       </c>
@@ -3228,7 +3276,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>102</v>
       </c>
@@ -3242,7 +3290,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>103</v>
       </c>
@@ -3256,7 +3304,7 @@
         <v>586.20000000000005</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>104</v>
       </c>
@@ -3270,7 +3318,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>105</v>
       </c>
@@ -3284,7 +3332,7 @@
         <v>266.39999999999998</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>106</v>
       </c>
@@ -3298,7 +3346,7 @@
         <v>39.4</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>107</v>
       </c>
@@ -3312,7 +3360,7 @@
         <v>39.4</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>108</v>
       </c>
@@ -3326,7 +3374,7 @@
         <v>39.4</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>109</v>
       </c>
@@ -3340,7 +3388,7 @@
         <v>58.2</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>110</v>
       </c>
@@ -3354,7 +3402,7 @@
         <v>88.9</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>111</v>
       </c>
@@ -3368,7 +3416,7 @@
         <v>88.9</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>112</v>
       </c>
@@ -3382,7 +3430,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>113</v>
       </c>
@@ -3396,7 +3444,7 @@
         <v>114.3</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>114</v>
       </c>
@@ -3410,7 +3458,7 @@
         <v>46.68</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>115</v>
       </c>
@@ -3424,7 +3472,7 @@
         <v>46.68</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>116</v>
       </c>
@@ -3438,7 +3486,7 @@
         <v>46.68</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>117</v>
       </c>
@@ -3452,7 +3500,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>118</v>
       </c>
@@ -3466,7 +3514,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>119</v>
       </c>
@@ -3480,7 +3528,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>120</v>
       </c>
@@ -3494,7 +3542,7 @@
         <v>90.8</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>121</v>
       </c>
@@ -3508,7 +3556,7 @@
         <v>90.8</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>122</v>
       </c>
@@ -3522,7 +3570,7 @@
         <v>71.87</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>123</v>
       </c>
@@ -3536,7 +3584,7 @@
         <v>101.5</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>124</v>
       </c>
@@ -3550,7 +3598,7 @@
         <v>37.700000000000003</v>
       </c>
     </row>
-    <row r="111" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A111" s="3" t="s">
         <v>125</v>
       </c>
@@ -3564,7 +3612,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>126</v>
       </c>
@@ -3578,7 +3626,7 @@
         <v>253.47</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>127</v>
       </c>
@@ -3592,7 +3640,7 @@
         <v>280.3</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>128</v>
       </c>
@@ -3606,7 +3654,7 @@
         <v>167.04</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>129</v>
       </c>
@@ -3620,7 +3668,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>130</v>
       </c>
@@ -3634,7 +3682,7 @@
         <v>176.4</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>131</v>
       </c>
@@ -3655,23 +3703,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="A100" sqref="A100"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="K102" sqref="K102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.44140625" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" customWidth="1"/>
-    <col min="17" max="17" width="11.33203125" style="6" customWidth="1"/>
-    <col min="18" max="18" width="18.88671875" customWidth="1"/>
-    <col min="19" max="19" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.453125" customWidth="1"/>
+    <col min="6" max="6" width="14.6328125" customWidth="1"/>
+    <col min="17" max="17" width="11.36328125" style="6" customWidth="1"/>
+    <col min="18" max="18" width="18.90625" customWidth="1"/>
+    <col min="19" max="19" width="31.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3727,7 +3775,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>154</v>
       </c>
@@ -3786,7 +3834,7 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>155</v>
       </c>
@@ -3845,7 +3893,7 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>156</v>
       </c>
@@ -3904,7 +3952,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>157</v>
       </c>
@@ -3963,7 +4011,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>163</v>
       </c>
@@ -4022,7 +4070,7 @@
         <v>1996</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>165</v>
       </c>
@@ -4084,7 +4132,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>166</v>
       </c>
@@ -4143,7 +4191,7 @@
         <v>1974</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>167</v>
       </c>
@@ -4202,7 +4250,7 @@
         <v>1974</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>168</v>
       </c>
@@ -4261,7 +4309,7 @@
         <v>1974</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>169</v>
       </c>
@@ -4320,7 +4368,7 @@
         <v>1974</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>170</v>
       </c>
@@ -4379,7 +4427,7 @@
         <v>1974</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>171</v>
       </c>
@@ -4438,7 +4486,7 @@
         <v>1974</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>172</v>
       </c>
@@ -4497,7 +4545,7 @@
         <v>1977</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>173</v>
       </c>
@@ -4556,7 +4604,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>174</v>
       </c>
@@ -4615,7 +4663,7 @@
         <v>1980</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>177</v>
       </c>
@@ -4674,7 +4722,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>178</v>
       </c>
@@ -4733,7 +4781,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>179</v>
       </c>
@@ -4792,7 +4840,7 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>180</v>
       </c>
@@ -4851,7 +4899,7 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>181</v>
       </c>
@@ -4910,7 +4958,7 @@
         <v>1996</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>182</v>
       </c>
@@ -4969,7 +5017,7 @@
         <v>1996</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>183</v>
       </c>
@@ -5028,7 +5076,7 @@
         <v>1996</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>184</v>
       </c>
@@ -5087,7 +5135,7 @@
         <v>1996</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>185</v>
       </c>
@@ -5146,7 +5194,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>186</v>
       </c>
@@ -5205,7 +5253,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>187</v>
       </c>
@@ -5264,7 +5312,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>188</v>
       </c>
@@ -5323,7 +5371,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>189</v>
       </c>
@@ -5382,7 +5430,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>190</v>
       </c>
@@ -5441,7 +5489,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>191</v>
       </c>
@@ -5500,7 +5548,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>192</v>
       </c>
@@ -5559,7 +5607,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>193</v>
       </c>
@@ -5618,7 +5666,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>194</v>
       </c>
@@ -5677,7 +5725,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>195</v>
       </c>
@@ -5736,7 +5784,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>196</v>
       </c>
@@ -5795,7 +5843,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>202</v>
       </c>
@@ -5854,7 +5902,7 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>203</v>
       </c>
@@ -5913,7 +5961,7 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>219</v>
       </c>
@@ -5975,7 +6023,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>220</v>
       </c>
@@ -6034,7 +6082,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>221</v>
       </c>
@@ -6093,7 +6141,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>222</v>
       </c>
@@ -6152,7 +6200,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>223</v>
       </c>
@@ -6211,7 +6259,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>224</v>
       </c>
@@ -6270,7 +6318,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>225</v>
       </c>
@@ -6329,7 +6377,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A46" s="4" t="s">
         <v>227</v>
       </c>
@@ -6391,7 +6439,7 @@
         <v>1972</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>228</v>
       </c>
@@ -6453,7 +6501,7 @@
         <v>1973</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>234</v>
       </c>
@@ -6512,7 +6560,7 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>235</v>
       </c>
@@ -6571,7 +6619,7 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>236</v>
       </c>
@@ -6630,7 +6678,7 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>238</v>
       </c>
@@ -6689,7 +6737,7 @@
         <v>1969</v>
       </c>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>239</v>
       </c>
@@ -6748,7 +6796,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>240</v>
       </c>
@@ -6807,7 +6855,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>241</v>
       </c>
@@ -6866,7 +6914,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>242</v>
       </c>
@@ -6925,7 +6973,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>243</v>
       </c>
@@ -6984,7 +7032,7 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>244</v>
       </c>
@@ -7043,7 +7091,7 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>245</v>
       </c>
@@ -7102,7 +7150,7 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>250</v>
       </c>
@@ -7161,7 +7209,7 @@
         <v>1981</v>
       </c>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>251</v>
       </c>
@@ -7220,7 +7268,7 @@
         <v>1981</v>
       </c>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>252</v>
       </c>
@@ -7279,7 +7327,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>253</v>
       </c>
@@ -7338,7 +7386,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>254</v>
       </c>
@@ -7397,7 +7445,7 @@
         <v>1984</v>
       </c>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>255</v>
       </c>
@@ -7456,7 +7504,7 @@
         <v>1984</v>
       </c>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>256</v>
       </c>
@@ -7515,7 +7563,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>257</v>
       </c>
@@ -7574,7 +7622,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>258</v>
       </c>
@@ -7633,7 +7681,7 @@
         <v>2004</v>
       </c>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>259</v>
       </c>
@@ -7692,7 +7740,7 @@
         <v>2004</v>
       </c>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>260</v>
       </c>
@@ -7751,7 +7799,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>261</v>
       </c>
@@ -7810,7 +7858,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>262</v>
       </c>
@@ -7869,7 +7917,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A72" s="4" t="s">
         <v>263</v>
       </c>
@@ -7928,7 +7976,7 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A73" s="4" t="s">
         <v>264</v>
       </c>
@@ -7990,7 +8038,7 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A74" s="4" t="s">
         <v>265</v>
       </c>
@@ -8049,7 +8097,7 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>267</v>
       </c>
@@ -8108,7 +8156,7 @@
         <v>1991</v>
       </c>
     </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>268</v>
       </c>
@@ -8167,7 +8215,7 @@
         <v>1991</v>
       </c>
     </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>269</v>
       </c>
@@ -8226,7 +8274,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>270</v>
       </c>
@@ -8288,7 +8336,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>271</v>
       </c>
@@ -8347,7 +8395,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>272</v>
       </c>
@@ -8406,7 +8454,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="81" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>273</v>
       </c>
@@ -8465,7 +8513,7 @@
         <v>1963</v>
       </c>
     </row>
-    <row r="82" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>275</v>
       </c>
@@ -8524,7 +8572,7 @@
         <v>1997</v>
       </c>
     </row>
-    <row r="83" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>276</v>
       </c>
@@ -8583,7 +8631,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="84" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>277</v>
       </c>
@@ -8642,7 +8690,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="85" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A85" s="4" t="s">
         <v>278</v>
       </c>
@@ -8701,7 +8749,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="86" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A86" s="4" t="s">
         <v>279</v>
       </c>
@@ -8760,7 +8808,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="87" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A87" s="4" t="s">
         <v>280</v>
       </c>
@@ -8819,7 +8867,7 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="88" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A88" s="4" t="s">
         <v>281</v>
       </c>
@@ -8878,7 +8926,7 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="89" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A89" s="4" t="s">
         <v>282</v>
       </c>
@@ -8937,7 +8985,7 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="90" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A90" s="4" t="s">
         <v>283</v>
       </c>
@@ -8999,7 +9047,7 @@
         <v>1969</v>
       </c>
     </row>
-    <row r="91" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>284</v>
       </c>
@@ -9058,7 +9106,7 @@
         <v>1981</v>
       </c>
     </row>
-    <row r="92" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>285</v>
       </c>
@@ -9117,7 +9165,7 @@
         <v>1981</v>
       </c>
     </row>
-    <row r="93" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>304</v>
       </c>
@@ -9164,7 +9212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>307</v>
       </c>
@@ -9208,7 +9256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>309</v>
       </c>
@@ -9255,7 +9303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>237</v>
       </c>
@@ -9315,7 +9363,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>312</v>
       </c>
@@ -9325,6 +9373,9 @@
       <c r="E97" t="s">
         <v>13</v>
       </c>
+      <c r="F97" s="8">
+        <v>2384.64013671875</v>
+      </c>
       <c r="G97">
         <v>0</v>
       </c>
@@ -9337,6 +9388,9 @@
       <c r="J97">
         <v>0</v>
       </c>
+      <c r="K97">
+        <v>561.16</v>
+      </c>
       <c r="L97">
         <v>1</v>
       </c>
@@ -9353,7 +9407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>313</v>
       </c>
@@ -9363,6 +9417,9 @@
       <c r="E98" t="s">
         <v>13</v>
       </c>
+      <c r="F98" s="8">
+        <v>2105</v>
+      </c>
       <c r="G98">
         <v>0</v>
       </c>
@@ -9375,6 +9432,9 @@
       <c r="J98">
         <v>0</v>
       </c>
+      <c r="K98">
+        <v>417.5</v>
+      </c>
       <c r="L98">
         <v>1</v>
       </c>
@@ -9391,7 +9451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>314</v>
       </c>
@@ -9401,6 +9461,9 @@
       <c r="E99" t="s">
         <v>13</v>
       </c>
+      <c r="F99" s="8">
+        <v>1829.8935546875</v>
+      </c>
       <c r="G99">
         <v>0</v>
       </c>
@@ -9413,6 +9476,9 @@
       <c r="J99">
         <v>0</v>
       </c>
+      <c r="K99">
+        <v>284.31837158203098</v>
+      </c>
       <c r="L99">
         <v>1</v>
       </c>
@@ -9429,7 +9495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>315</v>
       </c>
@@ -9439,6 +9505,9 @@
       <c r="E100" t="s">
         <v>13</v>
       </c>
+      <c r="F100" s="8">
+        <v>791.454833984375</v>
+      </c>
       <c r="G100">
         <v>0</v>
       </c>
@@ -9451,6 +9520,9 @@
       <c r="J100">
         <v>0</v>
       </c>
+      <c r="K100">
+        <v>0</v>
+      </c>
       <c r="L100">
         <v>1</v>
       </c>
@@ -9467,7 +9539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>316</v>
       </c>
@@ -9477,6 +9549,9 @@
       <c r="E101" t="s">
         <v>13</v>
       </c>
+      <c r="F101" s="8">
+        <v>0</v>
+      </c>
       <c r="G101">
         <v>0</v>
       </c>
@@ -9487,6 +9562,9 @@
         <v>0</v>
       </c>
       <c r="J101">
+        <v>0</v>
+      </c>
+      <c r="K101">
         <v>0</v>
       </c>
       <c r="L101">
@@ -9510,6 +9588,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -9521,9 +9600,9 @@
       <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>160</v>
       </c>
@@ -9543,7 +9622,7 @@
         <v>5.55</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>140</v>
       </c>
@@ -9560,7 +9639,7 @@
         <v>5.55</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>141</v>
       </c>
@@ -9577,7 +9656,7 @@
         <v>5.55</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>142</v>
       </c>
@@ -9594,7 +9673,7 @@
         <v>5.55</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>158</v>
       </c>
@@ -9611,7 +9690,7 @@
         <v>10.72</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>159</v>
       </c>
@@ -9628,7 +9707,7 @@
         <v>10.72</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>148</v>
       </c>
@@ -9645,7 +9724,7 @@
         <v>5.62</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>149</v>
       </c>
@@ -9662,7 +9741,7 @@
         <v>9.23</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>150</v>
       </c>
@@ -9679,7 +9758,7 @@
         <v>9.23</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>237</v>
       </c>
@@ -9716,9 +9795,9 @@
       <selection activeCell="A7" sqref="A7:XFD10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -9774,7 +9853,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>229</v>
       </c>
@@ -9834,7 +9913,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>230</v>
       </c>
@@ -9894,7 +9973,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>231</v>
       </c>
@@ -9951,7 +10030,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>232</v>
       </c>
@@ -10008,7 +10087,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>233</v>
       </c>
@@ -10065,7 +10144,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>246</v>
       </c>
@@ -10130,7 +10209,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>247</v>
       </c>
@@ -10189,7 +10268,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>248</v>
       </c>
@@ -10248,7 +10327,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>249</v>
       </c>
@@ -10320,9 +10399,9 @@
       <selection activeCell="A17" sqref="A17:XFD20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>217</v>
       </c>
@@ -10342,7 +10421,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>218</v>
       </c>
@@ -10362,7 +10441,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>204</v>
       </c>
@@ -10382,7 +10461,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>205</v>
       </c>
@@ -10402,7 +10481,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>206</v>
       </c>
@@ -10422,7 +10501,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>207</v>
       </c>
@@ -10442,7 +10521,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>208</v>
       </c>
@@ -10462,7 +10541,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>209</v>
       </c>
@@ -10482,7 +10561,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>210</v>
       </c>
@@ -10502,7 +10581,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>211</v>
       </c>
@@ -10522,7 +10601,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>212</v>
       </c>
@@ -10542,7 +10621,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>213</v>
       </c>
@@ -10562,7 +10641,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>214</v>
       </c>
@@ -10582,7 +10661,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>215</v>
       </c>
@@ -10602,7 +10681,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>175</v>
       </c>
@@ -10622,7 +10701,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>176</v>
       </c>
@@ -10642,7 +10721,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>197</v>
       </c>
@@ -10662,7 +10741,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>198</v>
       </c>
@@ -10682,7 +10761,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>199</v>
       </c>
@@ -10702,7 +10781,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>200</v>
       </c>

</xml_diff>

<commit_message>
cleaned up generator file
</commit_message>
<xml_diff>
--- a/PNW_generators.xlsx
+++ b/PNW_generators.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sdenaro\OneDrive - University of North Carolina at Chapel Hill\UNC_2017\Dispatch_model\PNW_Dispatch\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joy Hill\Desktop\BPA_stuff\PNW_Dispatch\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9190" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1097" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1105" uniqueCount="319">
   <si>
     <t>name</t>
   </si>
@@ -560,9 +560,6 @@
     <t>RUPERT_1002</t>
   </si>
   <si>
-    <t>CS</t>
-  </si>
-  <si>
     <t>ALDEN BAILEY_LOKI</t>
   </si>
   <si>
@@ -1020,6 +1017,12 @@
   </si>
   <si>
     <t>imports</t>
+  </si>
+  <si>
+    <t>nuc</t>
+  </si>
+  <si>
+    <t>ngst</t>
   </si>
 </sst>
 </file>
@@ -1691,7 +1694,7 @@
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns="" Requires="cx1">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="2" name="Chart 1"/>
@@ -1711,7 +1714,7 @@
       <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvPr id="2" name="Rectangle 1"/>
             <xdr:cNvSpPr>
               <a:spLocks noTextEdit="1"/>
             </xdr:cNvSpPr>
@@ -2017,12 +2020,12 @@
       <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.1796875" customWidth="1"/>
+    <col min="1" max="1" width="25.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2066,7 +2069,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -2080,7 +2083,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -2094,7 +2097,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -2108,7 +2111,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -2122,7 +2125,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -2136,7 +2139,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -2150,7 +2153,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -2164,7 +2167,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -2178,7 +2181,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -2192,7 +2195,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -2206,7 +2209,7 @@
         <v>30.9</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -2220,7 +2223,7 @@
         <v>30.9</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -2234,7 +2237,7 @@
         <v>179.4</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -2248,7 +2251,7 @@
         <v>122.1</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -2262,7 +2265,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -2276,7 +2279,7 @@
         <v>301.5</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -2290,7 +2293,7 @@
         <v>10.9</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -2304,7 +2307,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -2318,7 +2321,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -2332,7 +2335,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -2346,7 +2349,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -2360,7 +2363,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>37</v>
       </c>
@@ -2374,7 +2377,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>38</v>
       </c>
@@ -2388,7 +2391,7 @@
         <v>729.9</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -2402,7 +2405,7 @@
         <v>729.9</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>40</v>
       </c>
@@ -2416,7 +2419,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>41</v>
       </c>
@@ -2430,7 +2433,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>42</v>
       </c>
@@ -2444,7 +2447,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>43</v>
       </c>
@@ -2458,7 +2461,7 @@
         <v>1170</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>44</v>
       </c>
@@ -2472,7 +2475,7 @@
         <v>124.65</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>45</v>
       </c>
@@ -2486,7 +2489,7 @@
         <v>144.35</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>46</v>
       </c>
@@ -2500,7 +2503,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>47</v>
       </c>
@@ -2514,7 +2517,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>48</v>
       </c>
@@ -2528,7 +2531,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>49</v>
       </c>
@@ -2542,7 +2545,7 @@
         <v>212.5</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>50</v>
       </c>
@@ -2556,7 +2559,7 @@
         <v>212.5</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>51</v>
       </c>
@@ -2570,7 +2573,7 @@
         <v>264.39999999999998</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>52</v>
       </c>
@@ -2584,7 +2587,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>53</v>
       </c>
@@ -2598,7 +2601,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>54</v>
       </c>
@@ -2612,7 +2615,7 @@
         <v>161.5</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>55</v>
       </c>
@@ -2626,7 +2629,7 @@
         <v>161.5</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>56</v>
       </c>
@@ -2640,7 +2643,7 @@
         <v>178.5</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>57</v>
       </c>
@@ -2654,7 +2657,7 @@
         <v>29.4</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>58</v>
       </c>
@@ -2668,7 +2671,7 @@
         <v>29.4</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>59</v>
       </c>
@@ -2682,7 +2685,7 @@
         <v>29.4</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>60</v>
       </c>
@@ -2696,7 +2699,7 @@
         <v>29.4</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>61</v>
       </c>
@@ -2710,7 +2713,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>62</v>
       </c>
@@ -2724,7 +2727,7 @@
         <v>11.4</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>63</v>
       </c>
@@ -2738,7 +2741,7 @@
         <v>11.4</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>64</v>
       </c>
@@ -2752,7 +2755,7 @@
         <v>11.4</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>65</v>
       </c>
@@ -2766,7 +2769,7 @@
         <v>11.4</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>66</v>
       </c>
@@ -2780,7 +2783,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>67</v>
       </c>
@@ -2794,7 +2797,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>68</v>
       </c>
@@ -2808,7 +2811,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>69</v>
       </c>
@@ -2822,7 +2825,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>70</v>
       </c>
@@ -2836,7 +2839,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>71</v>
       </c>
@@ -2850,7 +2853,7 @@
         <v>-166</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>72</v>
       </c>
@@ -2864,7 +2867,7 @@
         <v>-166</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>73</v>
       </c>
@@ -2878,7 +2881,7 @@
         <v>-166</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>74</v>
       </c>
@@ -2892,7 +2895,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>75</v>
       </c>
@@ -2906,7 +2909,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>76</v>
       </c>
@@ -2920,7 +2923,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>77</v>
       </c>
@@ -2934,7 +2937,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>78</v>
       </c>
@@ -2948,7 +2951,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>79</v>
       </c>
@@ -2962,7 +2965,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>80</v>
       </c>
@@ -2976,7 +2979,7 @@
         <v>689.4</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>81</v>
       </c>
@@ -2990,7 +2993,7 @@
         <v>501.5</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>82</v>
       </c>
@@ -3004,7 +3007,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>83</v>
       </c>
@@ -3018,7 +3021,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>84</v>
       </c>
@@ -3032,7 +3035,7 @@
         <v>106.1</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>85</v>
       </c>
@@ -3046,7 +3049,7 @@
         <v>204.5</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>86</v>
       </c>
@@ -3060,7 +3063,7 @@
         <v>106.1</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>87</v>
       </c>
@@ -3074,7 +3077,7 @@
         <v>204.5</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>88</v>
       </c>
@@ -3094,7 +3097,7 @@
         <v>1956261</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>89</v>
       </c>
@@ -3108,7 +3111,7 @@
         <v>310.60000000000002</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>90</v>
       </c>
@@ -3122,7 +3125,7 @@
         <v>68.3</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>91</v>
       </c>
@@ -3136,7 +3139,7 @@
         <v>68.3</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>92</v>
       </c>
@@ -3150,7 +3153,7 @@
         <v>68.3</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>93</v>
       </c>
@@ -3164,7 +3167,7 @@
         <v>68.3</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>94</v>
       </c>
@@ -3178,7 +3181,7 @@
         <v>68.3</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>95</v>
       </c>
@@ -3192,7 +3195,7 @@
         <v>68.3</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>96</v>
       </c>
@@ -3206,7 +3209,7 @@
         <v>176.4</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>97</v>
       </c>
@@ -3220,7 +3223,7 @@
         <v>642.20000000000005</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>98</v>
       </c>
@@ -3234,7 +3237,7 @@
         <v>185.8</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>99</v>
       </c>
@@ -3248,7 +3251,7 @@
         <v>80.599999999999994</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>100</v>
       </c>
@@ -3262,7 +3265,7 @@
         <v>62.2</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>101</v>
       </c>
@@ -3276,7 +3279,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>102</v>
       </c>
@@ -3290,7 +3293,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>103</v>
       </c>
@@ -3304,7 +3307,7 @@
         <v>586.20000000000005</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>104</v>
       </c>
@@ -3318,7 +3321,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>105</v>
       </c>
@@ -3332,7 +3335,7 @@
         <v>266.39999999999998</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>106</v>
       </c>
@@ -3346,7 +3349,7 @@
         <v>39.4</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>107</v>
       </c>
@@ -3360,7 +3363,7 @@
         <v>39.4</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>108</v>
       </c>
@@ -3374,7 +3377,7 @@
         <v>39.4</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>109</v>
       </c>
@@ -3388,7 +3391,7 @@
         <v>58.2</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>110</v>
       </c>
@@ -3402,7 +3405,7 @@
         <v>88.9</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>111</v>
       </c>
@@ -3416,7 +3419,7 @@
         <v>88.9</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>112</v>
       </c>
@@ -3430,7 +3433,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>113</v>
       </c>
@@ -3444,7 +3447,7 @@
         <v>114.3</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>114</v>
       </c>
@@ -3458,7 +3461,7 @@
         <v>46.68</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>115</v>
       </c>
@@ -3472,7 +3475,7 @@
         <v>46.68</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>116</v>
       </c>
@@ -3486,7 +3489,7 @@
         <v>46.68</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>117</v>
       </c>
@@ -3500,7 +3503,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>118</v>
       </c>
@@ -3514,7 +3517,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>119</v>
       </c>
@@ -3528,7 +3531,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>120</v>
       </c>
@@ -3542,7 +3545,7 @@
         <v>90.8</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>121</v>
       </c>
@@ -3556,7 +3559,7 @@
         <v>90.8</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>122</v>
       </c>
@@ -3570,7 +3573,7 @@
         <v>71.87</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>123</v>
       </c>
@@ -3584,7 +3587,7 @@
         <v>101.5</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>124</v>
       </c>
@@ -3598,7 +3601,7 @@
         <v>37.700000000000003</v>
       </c>
     </row>
-    <row r="111" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A111" s="3" t="s">
         <v>125</v>
       </c>
@@ -3612,7 +3615,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>126</v>
       </c>
@@ -3626,7 +3629,7 @@
         <v>253.47</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>127</v>
       </c>
@@ -3640,7 +3643,7 @@
         <v>280.3</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>128</v>
       </c>
@@ -3654,7 +3657,7 @@
         <v>167.04</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>129</v>
       </c>
@@ -3668,7 +3671,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>130</v>
       </c>
@@ -3682,7 +3685,7 @@
         <v>176.4</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>131</v>
       </c>
@@ -3706,20 +3709,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="K102" sqref="K102"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B101" sqref="B101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.453125" customWidth="1"/>
-    <col min="6" max="6" width="14.6328125" customWidth="1"/>
-    <col min="17" max="17" width="11.36328125" style="6" customWidth="1"/>
-    <col min="18" max="18" width="18.90625" customWidth="1"/>
-    <col min="19" max="19" width="31.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.44140625" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" customWidth="1"/>
+    <col min="17" max="17" width="11.33203125" style="6" customWidth="1"/>
+    <col min="18" max="18" width="18.88671875" customWidth="1"/>
+    <col min="19" max="19" width="31.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3730,7 +3733,7 @@
         <v>146</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
@@ -3772,21 +3775,21 @@
         <v>145</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>154</v>
       </c>
       <c r="B2" t="s">
-        <v>153</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
         <v>134</v>
       </c>
       <c r="D2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E2" t="s">
         <v>13</v>
@@ -3834,18 +3837,18 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>155</v>
       </c>
       <c r="B3" t="s">
-        <v>153</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
         <v>134</v>
       </c>
       <c r="D3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E3" t="s">
         <v>13</v>
@@ -3893,18 +3896,18 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>156</v>
       </c>
       <c r="B4" t="s">
-        <v>161</v>
+        <v>132</v>
       </c>
       <c r="C4" t="s">
         <v>134</v>
       </c>
       <c r="D4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E4" t="s">
         <v>13</v>
@@ -3952,18 +3955,18 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>157</v>
       </c>
       <c r="B5" t="s">
-        <v>162</v>
+        <v>132</v>
       </c>
       <c r="C5" t="s">
         <v>134</v>
       </c>
       <c r="D5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E5" t="s">
         <v>13</v>
@@ -4011,18 +4014,18 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>163</v>
       </c>
       <c r="B6" t="s">
-        <v>164</v>
+        <v>132</v>
       </c>
       <c r="C6" t="s">
         <v>134</v>
       </c>
       <c r="D6" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E6" t="s">
         <v>13</v>
@@ -4070,18 +4073,18 @@
         <v>1996</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B7" t="s">
-        <v>153</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
         <v>134</v>
       </c>
       <c r="D7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E7" t="s">
         <v>13</v>
@@ -4126,24 +4129,24 @@
         <v>7.6</v>
       </c>
       <c r="R7" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="T7">
         <v>2001</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B8" t="s">
-        <v>161</v>
+        <v>132</v>
       </c>
       <c r="C8" t="s">
         <v>134</v>
       </c>
       <c r="D8" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E8" t="s">
         <v>13</v>
@@ -4191,18 +4194,18 @@
         <v>1974</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B9" t="s">
-        <v>161</v>
+        <v>132</v>
       </c>
       <c r="C9" t="s">
         <v>134</v>
       </c>
       <c r="D9" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E9" t="s">
         <v>13</v>
@@ -4250,18 +4253,18 @@
         <v>1974</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B10" t="s">
-        <v>161</v>
+        <v>132</v>
       </c>
       <c r="C10" t="s">
         <v>134</v>
       </c>
       <c r="D10" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E10" t="s">
         <v>13</v>
@@ -4309,18 +4312,18 @@
         <v>1974</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B11" t="s">
-        <v>161</v>
+        <v>132</v>
       </c>
       <c r="C11" t="s">
         <v>134</v>
       </c>
       <c r="D11" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E11" t="s">
         <v>13</v>
@@ -4368,18 +4371,18 @@
         <v>1974</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B12" t="s">
-        <v>161</v>
+        <v>132</v>
       </c>
       <c r="C12" t="s">
         <v>134</v>
       </c>
       <c r="D12" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E12" t="s">
         <v>13</v>
@@ -4427,18 +4430,18 @@
         <v>1974</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B13" t="s">
-        <v>161</v>
+        <v>132</v>
       </c>
       <c r="C13" t="s">
         <v>134</v>
       </c>
       <c r="D13" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E13" t="s">
         <v>13</v>
@@ -4486,18 +4489,18 @@
         <v>1974</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B14" t="s">
-        <v>162</v>
+        <v>132</v>
       </c>
       <c r="C14" t="s">
         <v>134</v>
       </c>
       <c r="D14" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E14" t="s">
         <v>13</v>
@@ -4545,18 +4548,18 @@
         <v>1977</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B15" t="s">
-        <v>153</v>
+        <v>20</v>
       </c>
       <c r="C15" t="s">
         <v>134</v>
       </c>
       <c r="D15" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E15" t="s">
         <v>13</v>
@@ -4604,12 +4607,12 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B16" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="C16" t="s">
         <v>133</v>
@@ -4663,18 +4666,18 @@
         <v>1980</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B17" t="s">
-        <v>161</v>
+        <v>132</v>
       </c>
       <c r="C17" t="s">
         <v>134</v>
       </c>
       <c r="D17" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E17" t="s">
         <v>13</v>
@@ -4722,18 +4725,18 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B18" t="s">
-        <v>162</v>
+        <v>132</v>
       </c>
       <c r="C18" t="s">
         <v>134</v>
       </c>
       <c r="D18" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E18" t="s">
         <v>13</v>
@@ -4781,18 +4784,18 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B19" t="s">
-        <v>161</v>
+        <v>132</v>
       </c>
       <c r="C19" t="s">
         <v>134</v>
       </c>
       <c r="D19" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E19" t="s">
         <v>13</v>
@@ -4840,18 +4843,18 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B20" t="s">
-        <v>162</v>
+        <v>132</v>
       </c>
       <c r="C20" t="s">
         <v>134</v>
       </c>
       <c r="D20" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E20" t="s">
         <v>13</v>
@@ -4899,18 +4902,18 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B21" t="s">
-        <v>162</v>
+        <v>132</v>
       </c>
       <c r="C21" t="s">
         <v>134</v>
       </c>
       <c r="D21" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E21" t="s">
         <v>13</v>
@@ -4958,18 +4961,18 @@
         <v>1996</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B22" t="s">
-        <v>161</v>
+        <v>132</v>
       </c>
       <c r="C22" t="s">
         <v>134</v>
       </c>
       <c r="D22" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E22" t="s">
         <v>13</v>
@@ -5017,18 +5020,18 @@
         <v>1996</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B23" t="s">
-        <v>162</v>
+        <v>132</v>
       </c>
       <c r="C23" t="s">
         <v>134</v>
       </c>
       <c r="D23" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E23" t="s">
         <v>13</v>
@@ -5076,18 +5079,18 @@
         <v>1996</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B24" t="s">
-        <v>161</v>
+        <v>132</v>
       </c>
       <c r="C24" t="s">
         <v>134</v>
       </c>
       <c r="D24" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E24" t="s">
         <v>13</v>
@@ -5135,18 +5138,18 @@
         <v>1996</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B25" t="s">
-        <v>161</v>
+        <v>132</v>
       </c>
       <c r="C25" t="s">
         <v>134</v>
       </c>
       <c r="D25" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E25" t="s">
         <v>13</v>
@@ -5194,18 +5197,18 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B26" t="s">
-        <v>161</v>
+        <v>132</v>
       </c>
       <c r="C26" t="s">
         <v>134</v>
       </c>
       <c r="D26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E26" t="s">
         <v>13</v>
@@ -5253,18 +5256,18 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:20" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B27" t="s">
-        <v>162</v>
+        <v>132</v>
       </c>
       <c r="C27" t="s">
         <v>134</v>
       </c>
       <c r="D27" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E27" t="s">
         <v>13</v>
@@ -5312,18 +5315,18 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B28" t="s">
-        <v>161</v>
+        <v>132</v>
       </c>
       <c r="C28" t="s">
         <v>134</v>
       </c>
       <c r="D28" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E28" t="s">
         <v>13</v>
@@ -5371,18 +5374,18 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B29" t="s">
-        <v>161</v>
+        <v>132</v>
       </c>
       <c r="C29" t="s">
         <v>134</v>
       </c>
       <c r="D29" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E29" t="s">
         <v>13</v>
@@ -5430,18 +5433,18 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B30" t="s">
-        <v>162</v>
+        <v>132</v>
       </c>
       <c r="C30" t="s">
         <v>134</v>
       </c>
       <c r="D30" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E30" t="s">
         <v>13</v>
@@ -5489,18 +5492,18 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B31" t="s">
-        <v>153</v>
+        <v>20</v>
       </c>
       <c r="C31" t="s">
         <v>134</v>
       </c>
       <c r="D31" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E31" t="s">
         <v>13</v>
@@ -5548,18 +5551,18 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B32" t="s">
-        <v>153</v>
+        <v>20</v>
       </c>
       <c r="C32" t="s">
         <v>134</v>
       </c>
       <c r="D32" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E32" t="s">
         <v>13</v>
@@ -5607,18 +5610,18 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B33" t="s">
-        <v>153</v>
+        <v>20</v>
       </c>
       <c r="C33" t="s">
         <v>134</v>
       </c>
       <c r="D33" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E33" t="s">
         <v>13</v>
@@ -5666,18 +5669,18 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B34" t="s">
-        <v>153</v>
+        <v>20</v>
       </c>
       <c r="C34" t="s">
         <v>134</v>
       </c>
       <c r="D34" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E34" t="s">
         <v>13</v>
@@ -5725,18 +5728,18 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B35" t="s">
-        <v>161</v>
+        <v>132</v>
       </c>
       <c r="C35" t="s">
         <v>134</v>
       </c>
       <c r="D35" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E35" t="s">
         <v>13</v>
@@ -5784,18 +5787,18 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B36" t="s">
-        <v>162</v>
+        <v>132</v>
       </c>
       <c r="C36" t="s">
         <v>134</v>
       </c>
       <c r="D36" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E36" t="s">
         <v>13</v>
@@ -5843,18 +5846,18 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B37" t="s">
-        <v>161</v>
+        <v>132</v>
       </c>
       <c r="C37" t="s">
         <v>134</v>
       </c>
       <c r="D37" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E37" t="s">
         <v>13</v>
@@ -5902,18 +5905,18 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B38" t="s">
-        <v>162</v>
+        <v>132</v>
       </c>
       <c r="C38" t="s">
         <v>134</v>
       </c>
       <c r="D38" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E38" t="s">
         <v>13</v>
@@ -5961,18 +5964,18 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B39" t="s">
-        <v>144</v>
+        <v>20</v>
       </c>
       <c r="C39" t="s">
         <v>136</v>
       </c>
       <c r="D39" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E39" t="s">
         <v>13</v>
@@ -6017,24 +6020,24 @@
         <v>10.4</v>
       </c>
       <c r="R39" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="T39">
         <v>2009</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B40" t="s">
-        <v>144</v>
+        <v>20</v>
       </c>
       <c r="C40" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D40" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E40" t="s">
         <v>13</v>
@@ -6082,18 +6085,18 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B41" t="s">
-        <v>144</v>
+        <v>20</v>
       </c>
       <c r="C41" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D41" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E41" t="s">
         <v>13</v>
@@ -6141,18 +6144,18 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B42" t="s">
-        <v>144</v>
+        <v>20</v>
       </c>
       <c r="C42" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D42" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E42" t="s">
         <v>13</v>
@@ -6200,18 +6203,18 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B43" t="s">
-        <v>144</v>
+        <v>20</v>
       </c>
       <c r="C43" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D43" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E43" t="s">
         <v>13</v>
@@ -6259,18 +6262,18 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B44" t="s">
-        <v>144</v>
+        <v>20</v>
       </c>
       <c r="C44" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D44" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E44" t="s">
         <v>13</v>
@@ -6318,18 +6321,18 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
+        <v>224</v>
+      </c>
+      <c r="B45" t="s">
+        <v>20</v>
+      </c>
+      <c r="C45" t="s">
         <v>225</v>
       </c>
-      <c r="B45" t="s">
-        <v>144</v>
-      </c>
-      <c r="C45" t="s">
-        <v>226</v>
-      </c>
       <c r="D45" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E45" t="s">
         <v>13</v>
@@ -6377,12 +6380,12 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B46" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="C46" t="s">
         <v>133</v>
@@ -6433,18 +6436,18 @@
         <v>10.1</v>
       </c>
       <c r="R46" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="T46">
         <v>1972</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B47" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="C47" t="s">
         <v>133</v>
@@ -6495,24 +6498,24 @@
         <v>10.1</v>
       </c>
       <c r="R47" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="T47">
         <v>1973</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B48" t="s">
-        <v>162</v>
+        <v>132</v>
       </c>
       <c r="C48" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D48" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E48" t="s">
         <v>13</v>
@@ -6560,18 +6563,18 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B49" t="s">
-        <v>161</v>
+        <v>132</v>
       </c>
       <c r="C49" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D49" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E49" t="s">
         <v>13</v>
@@ -6619,18 +6622,18 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B50" t="s">
-        <v>161</v>
+        <v>132</v>
       </c>
       <c r="C50" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D50" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E50" t="s">
         <v>13</v>
@@ -6678,18 +6681,18 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B51" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="C51" t="s">
         <v>136</v>
       </c>
       <c r="D51" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E51" t="s">
         <v>13</v>
@@ -6737,18 +6740,18 @@
         <v>1969</v>
       </c>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B52" t="s">
-        <v>161</v>
+        <v>132</v>
       </c>
       <c r="C52" t="s">
         <v>134</v>
       </c>
       <c r="D52" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E52" t="s">
         <v>13</v>
@@ -6796,18 +6799,18 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B53" t="s">
-        <v>161</v>
+        <v>132</v>
       </c>
       <c r="C53" t="s">
         <v>134</v>
       </c>
       <c r="D53" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E53" t="s">
         <v>13</v>
@@ -6855,18 +6858,18 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B54" t="s">
-        <v>161</v>
+        <v>132</v>
       </c>
       <c r="C54" t="s">
         <v>134</v>
       </c>
       <c r="D54" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E54" t="s">
         <v>13</v>
@@ -6914,18 +6917,18 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B55" t="s">
-        <v>162</v>
+        <v>132</v>
       </c>
       <c r="C55" t="s">
         <v>134</v>
       </c>
       <c r="D55" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E55" t="s">
         <v>13</v>
@@ -6973,18 +6976,18 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B56" t="s">
-        <v>161</v>
+        <v>132</v>
       </c>
       <c r="C56" t="s">
         <v>134</v>
       </c>
       <c r="D56" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E56" t="s">
         <v>13</v>
@@ -7032,18 +7035,18 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B57" t="s">
-        <v>161</v>
+        <v>132</v>
       </c>
       <c r="C57" t="s">
         <v>134</v>
       </c>
       <c r="D57" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E57" t="s">
         <v>13</v>
@@ -7091,18 +7094,18 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B58" t="s">
-        <v>162</v>
+        <v>132</v>
       </c>
       <c r="C58" t="s">
         <v>134</v>
       </c>
       <c r="D58" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E58" t="s">
         <v>13</v>
@@ -7150,18 +7153,18 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B59" t="s">
-        <v>153</v>
+        <v>20</v>
       </c>
       <c r="C59" t="s">
         <v>134</v>
       </c>
       <c r="D59" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E59" t="s">
         <v>13</v>
@@ -7209,18 +7212,18 @@
         <v>1981</v>
       </c>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B60" t="s">
-        <v>153</v>
+        <v>20</v>
       </c>
       <c r="C60" t="s">
         <v>134</v>
       </c>
       <c r="D60" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E60" t="s">
         <v>13</v>
@@ -7268,18 +7271,18 @@
         <v>1981</v>
       </c>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B61" t="s">
-        <v>161</v>
+        <v>132</v>
       </c>
       <c r="C61" t="s">
         <v>134</v>
       </c>
       <c r="D61" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E61" t="s">
         <v>13</v>
@@ -7327,18 +7330,18 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B62" t="s">
-        <v>162</v>
+        <v>132</v>
       </c>
       <c r="C62" t="s">
         <v>134</v>
       </c>
       <c r="D62" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E62" t="s">
         <v>13</v>
@@ -7386,18 +7389,18 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B63" t="s">
-        <v>153</v>
+        <v>20</v>
       </c>
       <c r="C63" t="s">
         <v>134</v>
       </c>
       <c r="D63" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E63" t="s">
         <v>13</v>
@@ -7445,18 +7448,18 @@
         <v>1984</v>
       </c>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B64" t="s">
-        <v>153</v>
+        <v>20</v>
       </c>
       <c r="C64" t="s">
         <v>134</v>
       </c>
       <c r="D64" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E64" t="s">
         <v>13</v>
@@ -7504,18 +7507,18 @@
         <v>1984</v>
       </c>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B65" t="s">
-        <v>153</v>
+        <v>20</v>
       </c>
       <c r="C65" t="s">
         <v>134</v>
       </c>
       <c r="D65" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E65" t="s">
         <v>13</v>
@@ -7563,18 +7566,18 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B66" t="s">
-        <v>153</v>
+        <v>20</v>
       </c>
       <c r="C66" t="s">
         <v>134</v>
       </c>
       <c r="D66" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E66" t="s">
         <v>13</v>
@@ -7622,18 +7625,18 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B67" t="s">
-        <v>161</v>
+        <v>132</v>
       </c>
       <c r="C67" t="s">
         <v>134</v>
       </c>
       <c r="D67" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E67" t="s">
         <v>13</v>
@@ -7681,18 +7684,18 @@
         <v>2004</v>
       </c>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B68" t="s">
-        <v>162</v>
+        <v>132</v>
       </c>
       <c r="C68" t="s">
         <v>134</v>
       </c>
       <c r="D68" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E68" t="s">
         <v>13</v>
@@ -7740,18 +7743,18 @@
         <v>2004</v>
       </c>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B69" t="s">
-        <v>161</v>
+        <v>132</v>
       </c>
       <c r="C69" t="s">
         <v>134</v>
       </c>
       <c r="D69" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E69" t="s">
         <v>13</v>
@@ -7799,18 +7802,18 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B70" t="s">
-        <v>161</v>
+        <v>132</v>
       </c>
       <c r="C70" t="s">
         <v>134</v>
       </c>
       <c r="D70" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E70" t="s">
         <v>13</v>
@@ -7858,18 +7861,18 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B71" t="s">
-        <v>162</v>
+        <v>132</v>
       </c>
       <c r="C71" t="s">
         <v>134</v>
       </c>
       <c r="D71" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E71" t="s">
         <v>13</v>
@@ -7917,18 +7920,18 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A72" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B72" t="s">
-        <v>144</v>
+        <v>20</v>
       </c>
       <c r="C72" t="s">
         <v>134</v>
       </c>
       <c r="D72" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E72" t="s">
         <v>13</v>
@@ -7976,18 +7979,18 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A73" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B73" t="s">
-        <v>144</v>
+        <v>20</v>
       </c>
       <c r="C73" t="s">
         <v>134</v>
       </c>
       <c r="D73" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E73" t="s">
         <v>13</v>
@@ -8032,24 +8035,24 @@
         <v>9.51</v>
       </c>
       <c r="R73" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="T73">
         <v>2005</v>
       </c>
     </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A74" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="B74" t="s">
+        <v>136</v>
+      </c>
+      <c r="C74" t="s">
         <v>265</v>
       </c>
-      <c r="B74" t="s">
-        <v>144</v>
-      </c>
-      <c r="C74" t="s">
-        <v>266</v>
-      </c>
       <c r="D74" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E74" t="s">
         <v>13</v>
@@ -8097,18 +8100,18 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B75" t="s">
-        <v>153</v>
+        <v>20</v>
       </c>
       <c r="C75" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D75" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E75" t="s">
         <v>13</v>
@@ -8156,18 +8159,18 @@
         <v>1991</v>
       </c>
     </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B76" t="s">
-        <v>153</v>
+        <v>20</v>
       </c>
       <c r="C76" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D76" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E76" t="s">
         <v>13</v>
@@ -8215,18 +8218,18 @@
         <v>1991</v>
       </c>
     </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B77" t="s">
-        <v>153</v>
+        <v>20</v>
       </c>
       <c r="C77" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D77" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E77" t="s">
         <v>13</v>
@@ -8274,18 +8277,18 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B78" t="s">
-        <v>162</v>
+        <v>132</v>
       </c>
       <c r="C78" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D78" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E78" t="s">
         <v>13</v>
@@ -8330,24 +8333,24 @@
         <v>5.72</v>
       </c>
       <c r="R78" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="T78">
         <v>1993</v>
       </c>
     </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B79" t="s">
-        <v>162</v>
+        <v>132</v>
       </c>
       <c r="C79" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D79" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E79" t="s">
         <v>13</v>
@@ -8395,18 +8398,18 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B80" t="s">
-        <v>161</v>
+        <v>132</v>
       </c>
       <c r="C80" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D80" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E80" t="s">
         <v>13</v>
@@ -8454,18 +8457,18 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="81" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B81" t="s">
-        <v>153</v>
+        <v>132</v>
       </c>
       <c r="C81" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D81" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E81" t="s">
         <v>13</v>
@@ -8513,18 +8516,18 @@
         <v>1963</v>
       </c>
     </row>
-    <row r="82" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B82" t="s">
-        <v>164</v>
+        <v>132</v>
       </c>
       <c r="C82" t="s">
         <v>134</v>
       </c>
       <c r="D82" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E82" t="s">
         <v>13</v>
@@ -8572,18 +8575,18 @@
         <v>1997</v>
       </c>
     </row>
-    <row r="83" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B83" t="s">
-        <v>161</v>
+        <v>132</v>
       </c>
       <c r="C83" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D83" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E83" t="s">
         <v>13</v>
@@ -8631,18 +8634,18 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="84" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B84" t="s">
-        <v>162</v>
+        <v>132</v>
       </c>
       <c r="C84" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D84" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E84" t="s">
         <v>13</v>
@@ -8690,18 +8693,18 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="85" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A85" s="4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B85" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="C85" t="s">
         <v>136</v>
       </c>
       <c r="D85" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E85" t="s">
         <v>13</v>
@@ -8749,18 +8752,18 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="86" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A86" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B86" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="C86" t="s">
         <v>136</v>
       </c>
       <c r="D86" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E86" t="s">
         <v>13</v>
@@ -8808,18 +8811,18 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="87" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A87" s="4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B87" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="C87" t="s">
         <v>136</v>
       </c>
       <c r="D87" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E87" t="s">
         <v>13</v>
@@ -8867,18 +8870,18 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="88" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A88" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B88" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="C88" t="s">
         <v>136</v>
       </c>
       <c r="D88" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E88" t="s">
         <v>13</v>
@@ -8926,18 +8929,18 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="89" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A89" s="4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B89" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="C89" t="s">
         <v>136</v>
       </c>
       <c r="D89" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E89" t="s">
         <v>13</v>
@@ -8985,18 +8988,18 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="90" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A90" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B90" t="s">
-        <v>143</v>
+        <v>318</v>
       </c>
       <c r="C90" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D90" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E90" t="s">
         <v>13</v>
@@ -9041,24 +9044,24 @@
         <v>9.51</v>
       </c>
       <c r="R90" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="T90">
         <v>1969</v>
       </c>
     </row>
-    <row r="91" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B91" t="s">
-        <v>153</v>
+        <v>20</v>
       </c>
       <c r="C91" t="s">
         <v>134</v>
       </c>
       <c r="D91" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E91" t="s">
         <v>13</v>
@@ -9106,18 +9109,18 @@
         <v>1981</v>
       </c>
     </row>
-    <row r="92" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B92" t="s">
-        <v>153</v>
+        <v>20</v>
       </c>
       <c r="C92" t="s">
         <v>134</v>
       </c>
       <c r="D92" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E92" t="s">
         <v>13</v>
@@ -9165,15 +9168,18 @@
         <v>1981</v>
       </c>
     </row>
-    <row r="93" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
+        <v>303</v>
+      </c>
+      <c r="B93" t="s">
+        <v>305</v>
+      </c>
+      <c r="C93" t="s">
         <v>304</v>
       </c>
-      <c r="C93" t="s">
+      <c r="D93" t="s">
         <v>305</v>
-      </c>
-      <c r="D93" t="s">
-        <v>306</v>
       </c>
       <c r="E93" t="s">
         <v>13</v>
@@ -9212,12 +9218,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
+        <v>306</v>
+      </c>
+      <c r="B94" t="s">
         <v>307</v>
       </c>
       <c r="D94" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E94" t="s">
         <v>13</v>
@@ -9256,15 +9265,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
+        <v>308</v>
+      </c>
+      <c r="B95" t="s">
         <v>309</v>
       </c>
       <c r="C95" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D95" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E95" t="s">
         <v>13</v>
@@ -9303,18 +9315,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B96" t="s">
-        <v>143</v>
+        <v>317</v>
       </c>
       <c r="C96" t="s">
         <v>135</v>
       </c>
       <c r="D96" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E96" t="s">
         <v>13</v>
@@ -9360,15 +9372,18 @@
         <v>0.91568000000000005</v>
       </c>
       <c r="S96" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="97" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A97" t="s">
-        <v>312</v>
+      <c r="B97" t="s">
+        <v>316</v>
       </c>
       <c r="D97" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E97" t="s">
         <v>13</v>
@@ -9407,12 +9422,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>313</v>
+        <v>312</v>
+      </c>
+      <c r="B98" t="s">
+        <v>316</v>
       </c>
       <c r="D98" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E98" t="s">
         <v>13</v>
@@ -9451,12 +9469,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>314</v>
+        <v>313</v>
+      </c>
+      <c r="B99" t="s">
+        <v>316</v>
       </c>
       <c r="D99" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E99" t="s">
         <v>13</v>
@@ -9495,12 +9516,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>315</v>
+        <v>314</v>
+      </c>
+      <c r="B100" t="s">
+        <v>316</v>
       </c>
       <c r="D100" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E100" t="s">
         <v>13</v>
@@ -9539,12 +9563,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
+        <v>315</v>
+      </c>
+      <c r="B101" t="s">
         <v>316</v>
       </c>
       <c r="D101" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E101" t="s">
         <v>13</v>
@@ -9600,9 +9627,9 @@
       <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>160</v>
       </c>
@@ -9622,7 +9649,7 @@
         <v>5.55</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>140</v>
       </c>
@@ -9639,7 +9666,7 @@
         <v>5.55</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>141</v>
       </c>
@@ -9656,7 +9683,7 @@
         <v>5.55</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>142</v>
       </c>
@@ -9673,7 +9700,7 @@
         <v>5.55</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>158</v>
       </c>
@@ -9690,7 +9717,7 @@
         <v>10.72</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>159</v>
       </c>
@@ -9707,7 +9734,7 @@
         <v>10.72</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>148</v>
       </c>
@@ -9724,7 +9751,7 @@
         <v>5.62</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>149</v>
       </c>
@@ -9741,7 +9768,7 @@
         <v>9.23</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>150</v>
       </c>
@@ -9758,9 +9785,9 @@
         <v>9.23</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B10" t="s">
         <v>143</v>
@@ -9795,9 +9822,9 @@
       <selection activeCell="A7" sqref="A7:XFD10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -9808,7 +9835,7 @@
         <v>146</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
@@ -9850,21 +9877,21 @@
         <v>145</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B2" t="s">
         <v>161</v>
       </c>
       <c r="C2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E2" t="s">
         <v>13</v>
@@ -9873,13 +9900,13 @@
         <v>60.5</v>
       </c>
       <c r="G2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="I2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="J2">
         <f>F2*0.4</f>
@@ -9899,7 +9926,7 @@
         <v>2</v>
       </c>
       <c r="O2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="P2">
         <f t="shared" ref="P2:P10" si="1">70*F2</f>
@@ -9907,24 +9934,24 @@
       </c>
       <c r="Q2" s="7"/>
       <c r="R2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="T2">
         <v>2002</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B3" t="s">
         <v>161</v>
       </c>
       <c r="C3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E3" t="s">
         <v>13</v>
@@ -9933,13 +9960,13 @@
         <v>60.5</v>
       </c>
       <c r="G3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="I3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="J3">
         <f>F3*0.4</f>
@@ -9959,7 +9986,7 @@
         <v>2</v>
       </c>
       <c r="O3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="P3">
         <f t="shared" si="1"/>
@@ -9967,24 +9994,24 @@
       </c>
       <c r="Q3" s="7"/>
       <c r="R3" s="4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="T3">
         <v>2002</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B4" t="s">
         <v>161</v>
       </c>
       <c r="C4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E4" t="s">
         <v>13</v>
@@ -9993,13 +10020,13 @@
         <v>60.5</v>
       </c>
       <c r="G4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="I4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="J4">
         <f>F4*0.4</f>
@@ -10019,7 +10046,7 @@
         <v>2</v>
       </c>
       <c r="O4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="P4">
         <f t="shared" si="1"/>
@@ -10030,18 +10057,18 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B5" t="s">
         <v>161</v>
       </c>
       <c r="C5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E5" t="s">
         <v>13</v>
@@ -10050,13 +10077,13 @@
         <v>60.5</v>
       </c>
       <c r="G5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="I5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="J5">
         <f>F5*0.4</f>
@@ -10076,7 +10103,7 @@
         <v>2</v>
       </c>
       <c r="O5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="P5">
         <f t="shared" si="1"/>
@@ -10087,18 +10114,18 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B6" t="s">
         <v>162</v>
       </c>
       <c r="C6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D6" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E6" t="s">
         <v>13</v>
@@ -10107,13 +10134,13 @@
         <v>80</v>
       </c>
       <c r="G6" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H6" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="I6" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="J6">
         <f>F6*0.4</f>
@@ -10133,7 +10160,7 @@
         <v>2</v>
       </c>
       <c r="O6" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="P6">
         <f t="shared" si="1"/>
@@ -10144,9 +10171,9 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B7" t="s">
         <v>153</v>
@@ -10155,7 +10182,7 @@
         <v>134</v>
       </c>
       <c r="D7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E7" t="s">
         <v>13</v>
@@ -10164,13 +10191,13 @@
         <v>11.4</v>
       </c>
       <c r="G7" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H7" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="I7" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="J7">
         <f>F7*0.35</f>
@@ -10190,28 +10217,28 @@
         <v>3.17</v>
       </c>
       <c r="O7" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="P7">
         <f t="shared" si="1"/>
         <v>798</v>
       </c>
       <c r="Q7" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="R7" t="s">
+        <v>290</v>
+      </c>
+      <c r="S7" t="s">
         <v>291</v>
-      </c>
-      <c r="S7" t="s">
-        <v>292</v>
       </c>
       <c r="T7">
         <v>2002</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B8" t="s">
         <v>153</v>
@@ -10220,7 +10247,7 @@
         <v>134</v>
       </c>
       <c r="D8" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E8" t="s">
         <v>13</v>
@@ -10229,13 +10256,13 @@
         <v>11.4</v>
       </c>
       <c r="G8" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H8" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="I8" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="J8">
         <f>F8*0.35</f>
@@ -10255,22 +10282,22 @@
         <v>3.17</v>
       </c>
       <c r="O8" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="P8">
         <f t="shared" si="1"/>
         <v>798</v>
       </c>
       <c r="Q8" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="T8">
         <v>2002</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B9" t="s">
         <v>153</v>
@@ -10279,7 +10306,7 @@
         <v>134</v>
       </c>
       <c r="D9" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E9" t="s">
         <v>13</v>
@@ -10288,13 +10315,13 @@
         <v>11.4</v>
       </c>
       <c r="G9" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H9" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="I9" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="J9">
         <f>F9*0.35</f>
@@ -10314,22 +10341,22 @@
         <v>3.17</v>
       </c>
       <c r="O9" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="P9">
         <f t="shared" si="1"/>
         <v>798</v>
       </c>
       <c r="Q9" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="T9">
         <v>2002</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B10" t="s">
         <v>153</v>
@@ -10338,7 +10365,7 @@
         <v>134</v>
       </c>
       <c r="D10" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E10" t="s">
         <v>13</v>
@@ -10347,13 +10374,13 @@
         <v>11.4</v>
       </c>
       <c r="G10" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H10" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="I10" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="J10">
         <f>F10*0.35</f>
@@ -10373,14 +10400,14 @@
         <v>3.17</v>
       </c>
       <c r="O10" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="P10">
         <f t="shared" si="1"/>
         <v>798</v>
       </c>
       <c r="Q10" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="T10">
         <v>2002</v>
@@ -10399,11 +10426,11 @@
       <selection activeCell="A17" sqref="A17:XFD20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B1" t="s">
         <v>161</v>
@@ -10418,12 +10445,12 @@
         <v>9.89</v>
       </c>
       <c r="R1" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B2" t="s">
         <v>162</v>
@@ -10438,12 +10465,12 @@
         <v>9.89</v>
       </c>
       <c r="R2" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B3" t="s">
         <v>144</v>
@@ -10458,12 +10485,12 @@
         <v>9.51</v>
       </c>
       <c r="R3" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B4" t="s">
         <v>144</v>
@@ -10478,12 +10505,12 @@
         <v>9.51</v>
       </c>
       <c r="R4" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B5" t="s">
         <v>144</v>
@@ -10498,12 +10525,12 @@
         <v>9.51</v>
       </c>
       <c r="R5" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B6" t="s">
         <v>144</v>
@@ -10518,12 +10545,12 @@
         <v>9.51</v>
       </c>
       <c r="R6" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B7" t="s">
         <v>144</v>
@@ -10538,12 +10565,12 @@
         <v>9.51</v>
       </c>
       <c r="R7" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B8" t="s">
         <v>144</v>
@@ -10558,12 +10585,12 @@
         <v>9.51</v>
       </c>
       <c r="R8" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B9" t="s">
         <v>144</v>
@@ -10578,12 +10605,12 @@
         <v>9.51</v>
       </c>
       <c r="R9" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B10" t="s">
         <v>144</v>
@@ -10598,12 +10625,12 @@
         <v>9.51</v>
       </c>
       <c r="R10" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B11" t="s">
         <v>144</v>
@@ -10618,12 +10645,12 @@
         <v>9.51</v>
       </c>
       <c r="R11" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B12" t="s">
         <v>144</v>
@@ -10638,12 +10665,12 @@
         <v>9.51</v>
       </c>
       <c r="R12" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B13" t="s">
         <v>144</v>
@@ -10658,12 +10685,12 @@
         <v>9.51</v>
       </c>
       <c r="R13" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B14" t="s">
         <v>144</v>
@@ -10678,12 +10705,12 @@
         <v>9.51</v>
       </c>
       <c r="R14" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B15" t="s">
         <v>161</v>
@@ -10698,12 +10725,12 @@
         <v>5.29</v>
       </c>
       <c r="R15" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B16" t="s">
         <v>162</v>
@@ -10718,12 +10745,12 @@
         <v>5.29</v>
       </c>
       <c r="R16" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B17" t="s">
         <v>153</v>
@@ -10735,15 +10762,15 @@
         <v>106</v>
       </c>
       <c r="P17" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="R17" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B18" t="s">
         <v>153</v>
@@ -10755,15 +10782,15 @@
         <v>106</v>
       </c>
       <c r="P18" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="R18" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B19" t="s">
         <v>153</v>
@@ -10775,15 +10802,15 @@
         <v>106</v>
       </c>
       <c r="P19" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="R19" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B20" t="s">
         <v>153</v>
@@ -10795,10 +10822,10 @@
         <v>106</v>
       </c>
       <c r="P20" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="R20" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
path 65 upramp/downramp fix
</commit_message>
<xml_diff>
--- a/PNW_generators.xlsx
+++ b/PNW_generators.xlsx
@@ -3707,7 +3707,7 @@
   <dimension ref="A1:T101"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="K102" sqref="K102"/>
+      <selection activeCell="K100" sqref="K100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9521,7 +9521,7 @@
         <v>0</v>
       </c>
       <c r="K100">
-        <v>0</v>
+        <v>135.980303955078</v>
       </c>
       <c r="L100">
         <v>1</v>

</xml_diff>

<commit_message>
update to generator and .dat file
</commit_message>
<xml_diff>
--- a/PNW_generators.xlsx
+++ b/PNW_generators.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sdenaro\OneDrive - University of North Carolina at Chapel Hill\UNC_2017\Dispatch_model\PNW_Dispatch\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joy Hill\Desktop\BPA_stuff\PNW_Dispatch\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9190" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,42 +31,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Lenovo User</author>
-  </authors>
-  <commentList>
-    <comment ref="A101" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Lenovo User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Maybe path 66 shouldn't be here because it's only exports</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1097" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1094" uniqueCount="317">
   <si>
     <t>name</t>
   </si>
@@ -1014,9 +980,6 @@
   </si>
   <si>
     <t>P65I</t>
-  </si>
-  <si>
-    <t>P66I</t>
   </si>
   <si>
     <t>imports</t>
@@ -1026,7 +989,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1062,19 +1025,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1691,7 +1641,7 @@
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns="" Requires="cx1">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="2" name="Chart 1"/>
@@ -1711,7 +1661,7 @@
       <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvPr id="2" name="Rectangle 1"/>
             <xdr:cNvSpPr>
               <a:spLocks noTextEdit="1"/>
             </xdr:cNvSpPr>
@@ -2017,12 +1967,12 @@
       <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.1796875" customWidth="1"/>
+    <col min="1" max="1" width="25.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2066,7 +2016,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -2080,7 +2030,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -2094,7 +2044,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -2108,7 +2058,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -2122,7 +2072,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -2136,7 +2086,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -2150,7 +2100,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -2164,7 +2114,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -2178,7 +2128,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -2192,7 +2142,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -2206,7 +2156,7 @@
         <v>30.9</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -2220,7 +2170,7 @@
         <v>30.9</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -2234,7 +2184,7 @@
         <v>179.4</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -2248,7 +2198,7 @@
         <v>122.1</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -2262,7 +2212,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -2276,7 +2226,7 @@
         <v>301.5</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -2290,7 +2240,7 @@
         <v>10.9</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -2304,7 +2254,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -2318,7 +2268,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -2332,7 +2282,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -2346,7 +2296,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -2360,7 +2310,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>37</v>
       </c>
@@ -2374,7 +2324,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>38</v>
       </c>
@@ -2388,7 +2338,7 @@
         <v>729.9</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -2402,7 +2352,7 @@
         <v>729.9</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>40</v>
       </c>
@@ -2416,7 +2366,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>41</v>
       </c>
@@ -2430,7 +2380,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>42</v>
       </c>
@@ -2444,7 +2394,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>43</v>
       </c>
@@ -2458,7 +2408,7 @@
         <v>1170</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>44</v>
       </c>
@@ -2472,7 +2422,7 @@
         <v>124.65</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>45</v>
       </c>
@@ -2486,7 +2436,7 @@
         <v>144.35</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>46</v>
       </c>
@@ -2500,7 +2450,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>47</v>
       </c>
@@ -2514,7 +2464,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>48</v>
       </c>
@@ -2528,7 +2478,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>49</v>
       </c>
@@ -2542,7 +2492,7 @@
         <v>212.5</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>50</v>
       </c>
@@ -2556,7 +2506,7 @@
         <v>212.5</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>51</v>
       </c>
@@ -2570,7 +2520,7 @@
         <v>264.39999999999998</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>52</v>
       </c>
@@ -2584,7 +2534,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>53</v>
       </c>
@@ -2598,7 +2548,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>54</v>
       </c>
@@ -2612,7 +2562,7 @@
         <v>161.5</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>55</v>
       </c>
@@ -2626,7 +2576,7 @@
         <v>161.5</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>56</v>
       </c>
@@ -2640,7 +2590,7 @@
         <v>178.5</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>57</v>
       </c>
@@ -2654,7 +2604,7 @@
         <v>29.4</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>58</v>
       </c>
@@ -2668,7 +2618,7 @@
         <v>29.4</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>59</v>
       </c>
@@ -2682,7 +2632,7 @@
         <v>29.4</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>60</v>
       </c>
@@ -2696,7 +2646,7 @@
         <v>29.4</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>61</v>
       </c>
@@ -2710,7 +2660,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>62</v>
       </c>
@@ -2724,7 +2674,7 @@
         <v>11.4</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>63</v>
       </c>
@@ -2738,7 +2688,7 @@
         <v>11.4</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>64</v>
       </c>
@@ -2752,7 +2702,7 @@
         <v>11.4</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>65</v>
       </c>
@@ -2766,7 +2716,7 @@
         <v>11.4</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>66</v>
       </c>
@@ -2780,7 +2730,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>67</v>
       </c>
@@ -2794,7 +2744,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>68</v>
       </c>
@@ -2808,7 +2758,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>69</v>
       </c>
@@ -2822,7 +2772,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>70</v>
       </c>
@@ -2836,7 +2786,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>71</v>
       </c>
@@ -2850,7 +2800,7 @@
         <v>-166</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>72</v>
       </c>
@@ -2864,7 +2814,7 @@
         <v>-166</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>73</v>
       </c>
@@ -2878,7 +2828,7 @@
         <v>-166</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>74</v>
       </c>
@@ -2892,7 +2842,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>75</v>
       </c>
@@ -2906,7 +2856,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>76</v>
       </c>
@@ -2920,7 +2870,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>77</v>
       </c>
@@ -2934,7 +2884,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>78</v>
       </c>
@@ -2948,7 +2898,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>79</v>
       </c>
@@ -2962,7 +2912,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>80</v>
       </c>
@@ -2976,7 +2926,7 @@
         <v>689.4</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>81</v>
       </c>
@@ -2990,7 +2940,7 @@
         <v>501.5</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>82</v>
       </c>
@@ -3004,7 +2954,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>83</v>
       </c>
@@ -3018,7 +2968,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>84</v>
       </c>
@@ -3032,7 +2982,7 @@
         <v>106.1</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>85</v>
       </c>
@@ -3046,7 +2996,7 @@
         <v>204.5</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>86</v>
       </c>
@@ -3060,7 +3010,7 @@
         <v>106.1</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>87</v>
       </c>
@@ -3074,7 +3024,7 @@
         <v>204.5</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>88</v>
       </c>
@@ -3094,7 +3044,7 @@
         <v>1956261</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>89</v>
       </c>
@@ -3108,7 +3058,7 @@
         <v>310.60000000000002</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>90</v>
       </c>
@@ -3122,7 +3072,7 @@
         <v>68.3</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>91</v>
       </c>
@@ -3136,7 +3086,7 @@
         <v>68.3</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>92</v>
       </c>
@@ -3150,7 +3100,7 @@
         <v>68.3</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>93</v>
       </c>
@@ -3164,7 +3114,7 @@
         <v>68.3</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>94</v>
       </c>
@@ -3178,7 +3128,7 @@
         <v>68.3</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>95</v>
       </c>
@@ -3192,7 +3142,7 @@
         <v>68.3</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>96</v>
       </c>
@@ -3206,7 +3156,7 @@
         <v>176.4</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>97</v>
       </c>
@@ -3220,7 +3170,7 @@
         <v>642.20000000000005</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>98</v>
       </c>
@@ -3234,7 +3184,7 @@
         <v>185.8</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>99</v>
       </c>
@@ -3248,7 +3198,7 @@
         <v>80.599999999999994</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>100</v>
       </c>
@@ -3262,7 +3212,7 @@
         <v>62.2</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>101</v>
       </c>
@@ -3276,7 +3226,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>102</v>
       </c>
@@ -3290,7 +3240,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>103</v>
       </c>
@@ -3304,7 +3254,7 @@
         <v>586.20000000000005</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>104</v>
       </c>
@@ -3318,7 +3268,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>105</v>
       </c>
@@ -3332,7 +3282,7 @@
         <v>266.39999999999998</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>106</v>
       </c>
@@ -3346,7 +3296,7 @@
         <v>39.4</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>107</v>
       </c>
@@ -3360,7 +3310,7 @@
         <v>39.4</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>108</v>
       </c>
@@ -3374,7 +3324,7 @@
         <v>39.4</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>109</v>
       </c>
@@ -3388,7 +3338,7 @@
         <v>58.2</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>110</v>
       </c>
@@ -3402,7 +3352,7 @@
         <v>88.9</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>111</v>
       </c>
@@ -3416,7 +3366,7 @@
         <v>88.9</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>112</v>
       </c>
@@ -3430,7 +3380,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>113</v>
       </c>
@@ -3444,7 +3394,7 @@
         <v>114.3</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>114</v>
       </c>
@@ -3458,7 +3408,7 @@
         <v>46.68</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>115</v>
       </c>
@@ -3472,7 +3422,7 @@
         <v>46.68</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>116</v>
       </c>
@@ -3486,7 +3436,7 @@
         <v>46.68</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>117</v>
       </c>
@@ -3500,7 +3450,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>118</v>
       </c>
@@ -3514,7 +3464,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>119</v>
       </c>
@@ -3528,7 +3478,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>120</v>
       </c>
@@ -3542,7 +3492,7 @@
         <v>90.8</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>121</v>
       </c>
@@ -3556,7 +3506,7 @@
         <v>90.8</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>122</v>
       </c>
@@ -3570,7 +3520,7 @@
         <v>71.87</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>123</v>
       </c>
@@ -3584,7 +3534,7 @@
         <v>101.5</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>124</v>
       </c>
@@ -3598,7 +3548,7 @@
         <v>37.700000000000003</v>
       </c>
     </row>
-    <row r="111" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A111" s="3" t="s">
         <v>125</v>
       </c>
@@ -3612,7 +3562,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>126</v>
       </c>
@@ -3626,7 +3576,7 @@
         <v>253.47</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>127</v>
       </c>
@@ -3640,7 +3590,7 @@
         <v>280.3</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>128</v>
       </c>
@@ -3654,7 +3604,7 @@
         <v>167.04</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>129</v>
       </c>
@@ -3668,7 +3618,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>130</v>
       </c>
@@ -3682,7 +3632,7 @@
         <v>176.4</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>131</v>
       </c>
@@ -3703,23 +3653,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T101"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="F100" sqref="F100"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="A100" sqref="A100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.453125" customWidth="1"/>
-    <col min="6" max="6" width="14.6328125" customWidth="1"/>
-    <col min="17" max="17" width="11.36328125" style="6" customWidth="1"/>
-    <col min="18" max="18" width="18.90625" customWidth="1"/>
-    <col min="19" max="19" width="31.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.44140625" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" customWidth="1"/>
+    <col min="17" max="17" width="11.33203125" style="6" customWidth="1"/>
+    <col min="18" max="18" width="18.88671875" customWidth="1"/>
+    <col min="19" max="19" width="31.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3775,7 +3725,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>154</v>
       </c>
@@ -3834,7 +3784,7 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>155</v>
       </c>
@@ -3893,7 +3843,7 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>156</v>
       </c>
@@ -3952,7 +3902,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>157</v>
       </c>
@@ -4011,7 +3961,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>163</v>
       </c>
@@ -4070,7 +4020,7 @@
         <v>1996</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>165</v>
       </c>
@@ -4132,7 +4082,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>166</v>
       </c>
@@ -4191,7 +4141,7 @@
         <v>1974</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>167</v>
       </c>
@@ -4250,7 +4200,7 @@
         <v>1974</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>168</v>
       </c>
@@ -4309,7 +4259,7 @@
         <v>1974</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>169</v>
       </c>
@@ -4368,7 +4318,7 @@
         <v>1974</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>170</v>
       </c>
@@ -4427,7 +4377,7 @@
         <v>1974</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>171</v>
       </c>
@@ -4486,7 +4436,7 @@
         <v>1974</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>172</v>
       </c>
@@ -4545,7 +4495,7 @@
         <v>1977</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>173</v>
       </c>
@@ -4604,7 +4554,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>174</v>
       </c>
@@ -4663,7 +4613,7 @@
         <v>1980</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>177</v>
       </c>
@@ -4722,7 +4672,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>178</v>
       </c>
@@ -4781,7 +4731,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>179</v>
       </c>
@@ -4840,7 +4790,7 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>180</v>
       </c>
@@ -4899,7 +4849,7 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>181</v>
       </c>
@@ -4958,7 +4908,7 @@
         <v>1996</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>182</v>
       </c>
@@ -5017,7 +4967,7 @@
         <v>1996</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>183</v>
       </c>
@@ -5076,7 +5026,7 @@
         <v>1996</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>184</v>
       </c>
@@ -5135,7 +5085,7 @@
         <v>1996</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>185</v>
       </c>
@@ -5194,7 +5144,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>186</v>
       </c>
@@ -5253,7 +5203,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:20" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>187</v>
       </c>
@@ -5312,7 +5262,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>188</v>
       </c>
@@ -5371,7 +5321,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>189</v>
       </c>
@@ -5430,7 +5380,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>190</v>
       </c>
@@ -5489,7 +5439,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>191</v>
       </c>
@@ -5548,7 +5498,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>192</v>
       </c>
@@ -5607,7 +5557,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>193</v>
       </c>
@@ -5666,7 +5616,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>194</v>
       </c>
@@ -5725,7 +5675,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>195</v>
       </c>
@@ -5784,7 +5734,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>196</v>
       </c>
@@ -5843,7 +5793,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>202</v>
       </c>
@@ -5902,7 +5852,7 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>203</v>
       </c>
@@ -5961,7 +5911,7 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>219</v>
       </c>
@@ -6023,7 +5973,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>220</v>
       </c>
@@ -6082,7 +6032,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>221</v>
       </c>
@@ -6141,7 +6091,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>222</v>
       </c>
@@ -6200,7 +6150,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>223</v>
       </c>
@@ -6259,7 +6209,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>224</v>
       </c>
@@ -6318,7 +6268,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>225</v>
       </c>
@@ -6377,7 +6327,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
         <v>227</v>
       </c>
@@ -6439,7 +6389,7 @@
         <v>1972</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>228</v>
       </c>
@@ -6501,7 +6451,7 @@
         <v>1973</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>234</v>
       </c>
@@ -6560,7 +6510,7 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>235</v>
       </c>
@@ -6619,7 +6569,7 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>236</v>
       </c>
@@ -6678,7 +6628,7 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>238</v>
       </c>
@@ -6737,7 +6687,7 @@
         <v>1969</v>
       </c>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>239</v>
       </c>
@@ -6796,7 +6746,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>240</v>
       </c>
@@ -6855,7 +6805,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>241</v>
       </c>
@@ -6914,7 +6864,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>242</v>
       </c>
@@ -6973,7 +6923,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>243</v>
       </c>
@@ -7032,7 +6982,7 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>244</v>
       </c>
@@ -7091,7 +7041,7 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>245</v>
       </c>
@@ -7150,7 +7100,7 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>250</v>
       </c>
@@ -7209,7 +7159,7 @@
         <v>1981</v>
       </c>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>251</v>
       </c>
@@ -7268,7 +7218,7 @@
         <v>1981</v>
       </c>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>252</v>
       </c>
@@ -7327,7 +7277,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>253</v>
       </c>
@@ -7386,7 +7336,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>254</v>
       </c>
@@ -7445,7 +7395,7 @@
         <v>1984</v>
       </c>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>255</v>
       </c>
@@ -7504,7 +7454,7 @@
         <v>1984</v>
       </c>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>256</v>
       </c>
@@ -7563,7 +7513,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>257</v>
       </c>
@@ -7622,7 +7572,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>258</v>
       </c>
@@ -7681,7 +7631,7 @@
         <v>2004</v>
       </c>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>259</v>
       </c>
@@ -7740,7 +7690,7 @@
         <v>2004</v>
       </c>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>260</v>
       </c>
@@ -7799,7 +7749,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>261</v>
       </c>
@@ -7858,7 +7808,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>262</v>
       </c>
@@ -7917,7 +7867,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A72" s="4" t="s">
         <v>263</v>
       </c>
@@ -7976,7 +7926,7 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A73" s="4" t="s">
         <v>264</v>
       </c>
@@ -8038,7 +7988,7 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A74" s="4" t="s">
         <v>265</v>
       </c>
@@ -8097,7 +8047,7 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>267</v>
       </c>
@@ -8156,7 +8106,7 @@
         <v>1991</v>
       </c>
     </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>268</v>
       </c>
@@ -8215,7 +8165,7 @@
         <v>1991</v>
       </c>
     </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>269</v>
       </c>
@@ -8274,7 +8224,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>270</v>
       </c>
@@ -8336,7 +8286,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>271</v>
       </c>
@@ -8395,7 +8345,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>272</v>
       </c>
@@ -8454,7 +8404,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="81" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>273</v>
       </c>
@@ -8513,7 +8463,7 @@
         <v>1963</v>
       </c>
     </row>
-    <row r="82" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>275</v>
       </c>
@@ -8572,7 +8522,7 @@
         <v>1997</v>
       </c>
     </row>
-    <row r="83" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>276</v>
       </c>
@@ -8631,7 +8581,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="84" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>277</v>
       </c>
@@ -8690,7 +8640,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="85" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A85" s="4" t="s">
         <v>278</v>
       </c>
@@ -8749,7 +8699,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="86" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A86" s="4" t="s">
         <v>279</v>
       </c>
@@ -8808,7 +8758,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="87" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A87" s="4" t="s">
         <v>280</v>
       </c>
@@ -8867,7 +8817,7 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="88" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A88" s="4" t="s">
         <v>281</v>
       </c>
@@ -8926,7 +8876,7 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="89" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A89" s="4" t="s">
         <v>282</v>
       </c>
@@ -8985,7 +8935,7 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="90" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A90" s="4" t="s">
         <v>283</v>
       </c>
@@ -9047,7 +8997,7 @@
         <v>1969</v>
       </c>
     </row>
-    <row r="91" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>284</v>
       </c>
@@ -9106,7 +9056,7 @@
         <v>1981</v>
       </c>
     </row>
-    <row r="92" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>285</v>
       </c>
@@ -9165,7 +9115,7 @@
         <v>1981</v>
       </c>
     </row>
-    <row r="93" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>304</v>
       </c>
@@ -9212,7 +9162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>307</v>
       </c>
@@ -9256,7 +9206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>309</v>
       </c>
@@ -9303,7 +9253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>237</v>
       </c>
@@ -9363,12 +9313,12 @@
         <v>311</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>312</v>
       </c>
       <c r="D97" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E97" t="s">
         <v>13</v>
@@ -9407,12 +9357,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>313</v>
       </c>
       <c r="D98" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E98" t="s">
         <v>13</v>
@@ -9451,12 +9401,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>314</v>
       </c>
       <c r="D99" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E99" t="s">
         <v>13</v>
@@ -9495,12 +9445,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>315</v>
       </c>
       <c r="D100" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E100" t="s">
         <v>13</v>
@@ -9536,50 +9486,6 @@
         <v>0</v>
       </c>
       <c r="P100">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A101" t="s">
-        <v>316</v>
-      </c>
-      <c r="D101" t="s">
-        <v>317</v>
-      </c>
-      <c r="E101" t="s">
-        <v>13</v>
-      </c>
-      <c r="F101" s="8">
-        <v>0</v>
-      </c>
-      <c r="G101">
-        <v>0</v>
-      </c>
-      <c r="H101">
-        <v>0</v>
-      </c>
-      <c r="I101">
-        <v>0</v>
-      </c>
-      <c r="J101">
-        <v>0</v>
-      </c>
-      <c r="K101">
-        <v>0</v>
-      </c>
-      <c r="L101">
-        <v>1</v>
-      </c>
-      <c r="M101">
-        <v>1</v>
-      </c>
-      <c r="N101">
-        <v>0</v>
-      </c>
-      <c r="O101">
-        <v>0</v>
-      </c>
-      <c r="P101">
         <v>0</v>
       </c>
     </row>
@@ -9588,7 +9494,6 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -9600,9 +9505,9 @@
       <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>160</v>
       </c>
@@ -9622,7 +9527,7 @@
         <v>5.55</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>140</v>
       </c>
@@ -9639,7 +9544,7 @@
         <v>5.55</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>141</v>
       </c>
@@ -9656,7 +9561,7 @@
         <v>5.55</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>142</v>
       </c>
@@ -9673,7 +9578,7 @@
         <v>5.55</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>158</v>
       </c>
@@ -9690,7 +9595,7 @@
         <v>10.72</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>159</v>
       </c>
@@ -9707,7 +9612,7 @@
         <v>10.72</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>148</v>
       </c>
@@ -9724,7 +9629,7 @@
         <v>5.62</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>149</v>
       </c>
@@ -9741,7 +9646,7 @@
         <v>9.23</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>150</v>
       </c>
@@ -9758,7 +9663,7 @@
         <v>9.23</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>237</v>
       </c>
@@ -9795,9 +9700,9 @@
       <selection activeCell="A7" sqref="A7:XFD10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -9853,7 +9758,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>229</v>
       </c>
@@ -9913,7 +9818,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>230</v>
       </c>
@@ -9973,7 +9878,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>231</v>
       </c>
@@ -10030,7 +9935,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>232</v>
       </c>
@@ -10087,7 +9992,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>233</v>
       </c>
@@ -10144,7 +10049,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>246</v>
       </c>
@@ -10209,7 +10114,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>247</v>
       </c>
@@ -10268,7 +10173,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>248</v>
       </c>
@@ -10327,7 +10232,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>249</v>
       </c>
@@ -10399,9 +10304,9 @@
       <selection activeCell="A17" sqref="A17:XFD20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>217</v>
       </c>
@@ -10421,7 +10326,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>218</v>
       </c>
@@ -10441,7 +10346,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>204</v>
       </c>
@@ -10461,7 +10366,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>205</v>
       </c>
@@ -10481,7 +10386,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>206</v>
       </c>
@@ -10501,7 +10406,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>207</v>
       </c>
@@ -10521,7 +10426,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>208</v>
       </c>
@@ -10541,7 +10446,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>209</v>
       </c>
@@ -10561,7 +10466,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>210</v>
       </c>
@@ -10581,7 +10486,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>211</v>
       </c>
@@ -10601,7 +10506,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>212</v>
       </c>
@@ -10621,7 +10526,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>213</v>
       </c>
@@ -10641,7 +10546,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>214</v>
       </c>
@@ -10661,7 +10566,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>215</v>
       </c>
@@ -10681,7 +10586,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>175</v>
       </c>
@@ -10701,7 +10606,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>176</v>
       </c>
@@ -10721,7 +10626,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>197</v>
       </c>
@@ -10741,7 +10646,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>198</v>
       </c>
@@ -10761,7 +10666,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>199</v>
       </c>
@@ -10781,7 +10686,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>200</v>
       </c>

</xml_diff>